<commit_message>
cleared files/added additional files for automation
</commit_message>
<xml_diff>
--- a/sm_core/Excel_Files/no_ports_test.xlsx
+++ b/sm_core/Excel_Files/no_ports_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sm-core\sm_core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backup\portfolio\sm_core\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2E3A4-C91F-4A9B-BD8C-6977AF8BCCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B2BF3-B4AB-4F88-9637-5FA91E0BEDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no_ports.xlsx" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>bd_account_id</t>
   </si>
@@ -59,36 +59,6 @@
   </si>
   <si>
     <t>bd_portfolio_id</t>
-  </si>
-  <si>
-    <t>TD Ameritrade</t>
-  </si>
-  <si>
-    <t>z053090</t>
-  </si>
-  <si>
-    <t>ROLLOVER IRA</t>
-  </si>
-  <si>
-    <t>HEIDI GUNDLACH</t>
-  </si>
-  <si>
-    <t>A456</t>
-  </si>
-  <si>
-    <t>Gundlach</t>
-  </si>
-  <si>
-    <t>Heidi</t>
-  </si>
-  <si>
-    <t>Gundlach, Heidi</t>
-  </si>
-  <si>
-    <t>Heidi Gundlach</t>
-  </si>
-  <si>
-    <t>z0525538961</t>
   </si>
 </sst>
 </file>
@@ -946,7 +916,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,39 +978,15 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1">
-        <v>943398813</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>